<commit_message>
accuracy of the three models
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="AM5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2541,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="AL15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM15" t="n">
         <v>1</v>
@@ -8756,7 +8756,7 @@
         <v>1</v>
       </c>
       <c r="AM61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -9285,7 +9285,7 @@
         <v>1</v>
       </c>
       <c r="AL65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM65" t="n">
         <v>1</v>
@@ -10089,7 +10089,7 @@
         <v>0</v>
       </c>
       <c r="AL71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM71" t="n">
         <v>0</v>
@@ -10625,7 +10625,7 @@
         <v>1</v>
       </c>
       <c r="AL75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM75" t="n">
         <v>1</v>
@@ -10763,7 +10763,7 @@
         <v>1</v>
       </c>
       <c r="AM76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -12388,7 +12388,7 @@
         <v>1</v>
       </c>
       <c r="AL88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM88" t="n">
         <v>1</v>
@@ -12669,7 +12669,7 @@
         <v>1</v>
       </c>
       <c r="AM90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -13204,7 +13204,7 @@
         <v>1</v>
       </c>
       <c r="AL94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM94" t="n">
         <v>1</v>
@@ -13482,10 +13482,10 @@
         <v>1</v>
       </c>
       <c r="AL96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -13623,7 +13623,7 @@
         <v>1</v>
       </c>
       <c r="AL97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM97" t="n">
         <v>1</v>
@@ -13763,7 +13763,7 @@
         <v>1</v>
       </c>
       <c r="AM98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -14018,7 +14018,7 @@
         <v>0</v>
       </c>
       <c r="AL100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM100" t="n">
         <v>0</v>
@@ -14152,7 +14152,7 @@
         <v>1</v>
       </c>
       <c r="AM101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -14821,9 +14821,7 @@
       <c r="AK106" t="n">
         <v>1</v>
       </c>
-      <c r="AL106" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL106" t="inlineStr"/>
       <c r="AM106" t="n">
         <v>1</v>
       </c>
@@ -14966,9 +14964,7 @@
       <c r="AK107" t="n">
         <v>1</v>
       </c>
-      <c r="AL107" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL107" t="inlineStr"/>
       <c r="AM107" t="n">
         <v>1</v>
       </c>
@@ -15101,9 +15097,7 @@
       <c r="AK108" t="n">
         <v>1</v>
       </c>
-      <c r="AL108" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL108" t="inlineStr"/>
       <c r="AM108" t="n">
         <v>1</v>
       </c>
@@ -15244,9 +15238,7 @@
       <c r="AK109" t="n">
         <v>1</v>
       </c>
-      <c r="AL109" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL109" t="inlineStr"/>
       <c r="AM109" t="n">
         <v>1</v>
       </c>
@@ -15385,9 +15377,7 @@
       <c r="AK110" t="n">
         <v>1</v>
       </c>
-      <c r="AL110" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL110" t="inlineStr"/>
       <c r="AM110" t="n">
         <v>1</v>
       </c>

</xml_diff>